<commit_message>
Fix some issues in the mtg from raw xlsx files
</commit_message>
<xml_diff>
--- a/0-data/0-raw/tree2c.xlsx
+++ b/0-data/0-raw/tree2c.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohamed\Desktop\terrain_mesures_millan2020\arbres_mtg\arbre2\A2C\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ciradfr.sharepoint.com/sites/AMAP-FSPM/Documents partages/Analyses/Allometries/0-data/0-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="A2C" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -209,7 +209,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -576,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -993,10 +993,10 @@
       <c r="U39" s="2"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="D40" s="3" t="s">
+      <c r="B40" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F40" s="5"/>
+      <c r="D40" s="5"/>
       <c r="G40" s="5"/>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
@@ -1006,10 +1006,10 @@
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="D41" t="s">
+      <c r="B41" t="s">
         <v>37</v>
       </c>
-      <c r="F41" s="5"/>
+      <c r="D41" s="5"/>
       <c r="G41" s="5">
         <v>24.8</v>
       </c>
@@ -1054,10 +1054,10 @@
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="E42" s="4" t="s">
+      <c r="C42" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F42" s="5"/>
+      <c r="D42" s="5"/>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
@@ -1067,10 +1067,10 @@
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="E43" t="s">
+      <c r="C43" t="s">
         <v>37</v>
       </c>
-      <c r="F43" s="5"/>
+      <c r="D43" s="5"/>
       <c r="G43" s="8">
         <v>24.5</v>
       </c>
@@ -1115,10 +1115,10 @@
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="D44" t="s">
+      <c r="B44" t="s">
         <v>38</v>
       </c>
-      <c r="F44" s="5"/>
+      <c r="D44" s="5"/>
       <c r="G44" s="5">
         <v>33</v>
       </c>
@@ -1132,10 +1132,10 @@
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="E45" s="4" t="s">
+      <c r="C45" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F45" s="5"/>
+      <c r="D45" s="5"/>
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
@@ -1145,10 +1145,10 @@
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="E46" t="s">
+      <c r="C46" t="s">
         <v>37</v>
       </c>
-      <c r="F46" s="5"/>
+      <c r="D46" s="5"/>
       <c r="G46" s="8">
         <v>70.5</v>
       </c>
@@ -1162,10 +1162,10 @@
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="D47" t="s">
+      <c r="B47" t="s">
         <v>40</v>
       </c>
-      <c r="F47" s="5"/>
+      <c r="D47" s="5"/>
       <c r="G47" s="5">
         <v>2.2999999999999998</v>
       </c>
@@ -1179,10 +1179,10 @@
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="E48" s="4" t="s">
+      <c r="C48" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F48" s="5"/>
+      <c r="D48" s="5"/>
       <c r="G48" s="5"/>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
@@ -1191,11 +1191,11 @@
         <v>2054</v>
       </c>
     </row>
-    <row r="49" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="E49" t="s">
+    <row r="49" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
         <v>37</v>
       </c>
-      <c r="F49" s="5"/>
+      <c r="D49" s="5"/>
       <c r="G49" s="8">
         <v>4</v>
       </c>
@@ -1208,11 +1208,11 @@
         <v>2055</v>
       </c>
     </row>
-    <row r="50" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D50" t="s">
+    <row r="50" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
         <v>41</v>
       </c>
-      <c r="F50" s="5"/>
+      <c r="D50" s="5"/>
       <c r="G50" s="5">
         <v>10.5</v>
       </c>
@@ -1256,11 +1256,11 @@
         <v>2.1231999999999998</v>
       </c>
     </row>
-    <row r="51" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="E51" s="4" t="s">
+    <row r="51" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="C51" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F51" s="5"/>
+      <c r="D51" s="5"/>
       <c r="G51" s="5"/>
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
@@ -1269,11 +1269,11 @@
         <v>2057</v>
       </c>
     </row>
-    <row r="52" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="E52" t="s">
+    <row r="52" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
         <v>37</v>
       </c>
-      <c r="F52" s="5"/>
+      <c r="D52" s="5"/>
       <c r="G52" s="8">
         <v>67</v>
       </c>
@@ -1317,11 +1317,11 @@
         <v>0.85820000000000007</v>
       </c>
     </row>
-    <row r="53" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D53" t="s">
+    <row r="53" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
         <v>42</v>
       </c>
-      <c r="F53" s="5"/>
+      <c r="D53" s="5"/>
       <c r="G53" s="5">
         <v>19.600000000000001</v>
       </c>
@@ -1365,11 +1365,11 @@
         <v>2.2835000000000001</v>
       </c>
     </row>
-    <row r="54" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="E54" s="4" t="s">
+    <row r="54" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="C54" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F54" s="5"/>
+      <c r="D54" s="5"/>
       <c r="G54" s="5"/>
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
@@ -1378,11 +1378,11 @@
         <v>2060</v>
       </c>
     </row>
-    <row r="55" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="E55" t="s">
+    <row r="55" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
         <v>37</v>
       </c>
-      <c r="F55" s="5"/>
+      <c r="D55" s="5"/>
       <c r="G55" s="8">
         <v>3.5</v>
       </c>
@@ -1395,11 +1395,11 @@
         <v>2061</v>
       </c>
     </row>
-    <row r="56" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D56" t="s">
+    <row r="56" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
         <v>43</v>
       </c>
-      <c r="F56" s="5"/>
+      <c r="D56" s="5"/>
       <c r="G56" s="5">
         <v>7</v>
       </c>
@@ -1412,11 +1412,11 @@
         <v>2062</v>
       </c>
     </row>
-    <row r="57" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="E57" s="4" t="s">
+    <row r="57" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="C57" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F57" s="5"/>
+      <c r="D57" s="5"/>
       <c r="G57" s="5"/>
       <c r="H57" s="5"/>
       <c r="I57" s="7"/>
@@ -1425,11 +1425,11 @@
         <v>2063</v>
       </c>
     </row>
-    <row r="58" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="E58" t="s">
+    <row r="58" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="C58" t="s">
         <v>37</v>
       </c>
-      <c r="F58" s="5"/>
+      <c r="D58" s="5"/>
       <c r="G58" s="8">
         <v>46.5</v>
       </c>
@@ -1442,11 +1442,11 @@
         <v>2064</v>
       </c>
     </row>
-    <row r="59" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D59" t="s">
+    <row r="59" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
         <v>44</v>
       </c>
-      <c r="F59" s="5"/>
+      <c r="D59" s="5"/>
       <c r="G59" s="5">
         <v>20.399999999999999</v>
       </c>
@@ -1459,11 +1459,11 @@
         <v>2065</v>
       </c>
     </row>
-    <row r="60" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="E60" s="4" t="s">
+    <row r="60" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="C60" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F60" s="5"/>
+      <c r="D60" s="5"/>
       <c r="G60" s="5"/>
       <c r="H60" s="5"/>
       <c r="I60" s="7"/>
@@ -1472,11 +1472,11 @@
         <v>2066</v>
       </c>
     </row>
-    <row r="61" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="E61" t="s">
+    <row r="61" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="C61" t="s">
         <v>37</v>
       </c>
-      <c r="F61" s="5"/>
+      <c r="D61" s="5"/>
       <c r="G61" s="8">
         <v>117.5</v>
       </c>
@@ -1520,11 +1520,11 @@
         <v>1.8706</v>
       </c>
     </row>
-    <row r="62" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D62" t="s">
+    <row r="62" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
         <v>45</v>
       </c>
-      <c r="F62" s="5"/>
+      <c r="D62" s="5"/>
       <c r="G62" s="5">
         <v>9</v>
       </c>
@@ -1568,11 +1568,11 @@
         <v>1.4581999999999999</v>
       </c>
     </row>
-    <row r="63" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="E63" s="4" t="s">
+    <row r="63" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="C63" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F63" s="5"/>
+      <c r="D63" s="5"/>
       <c r="G63" s="5"/>
       <c r="H63" s="5"/>
       <c r="I63" s="7"/>
@@ -1581,11 +1581,11 @@
         <v>2069</v>
       </c>
     </row>
-    <row r="64" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="E64" t="s">
+    <row r="64" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="C64" t="s">
         <v>37</v>
       </c>
-      <c r="F64" s="5"/>
+      <c r="D64" s="5"/>
       <c r="G64" s="8">
         <v>84.5</v>
       </c>
@@ -1598,11 +1598,11 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="65" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D65" t="s">
+    <row r="65" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
         <v>46</v>
       </c>
-      <c r="F65" s="5"/>
+      <c r="D65" s="5"/>
       <c r="G65" s="5">
         <v>118</v>
       </c>
@@ -1646,7 +1646,7 @@
         <v>0.75349999999999995</v>
       </c>
     </row>
-    <row r="66" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:21" x14ac:dyDescent="0.3">
       <c r="D66" s="5"/>
       <c r="E66" s="6"/>
       <c r="F66" s="5"/>
@@ -1655,7 +1655,7 @@
       <c r="I66" s="7"/>
       <c r="J66" s="5"/>
     </row>
-    <row r="67" spans="4:21" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:21" x14ac:dyDescent="0.3">
       <c r="D67" s="5"/>
       <c r="E67" s="5"/>
       <c r="F67" s="5"/>
@@ -1671,6 +1671,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D817E2E441AD8840AD152F485CF91FFD" ma:contentTypeVersion="2" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="9bd92fc451d28d7a43c1e2d68c8f297e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f3bb3ef3-874e-4bfe-a810-81c575a8e62c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6122410798bbeb3d5138414ef9c1dd21" ns2:_="">
     <xsd:import namespace="f3bb3ef3-874e-4bfe-a810-81c575a8e62c"/>
@@ -1802,15 +1811,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1818,13 +1818,43 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{345E4A68-49FF-4A84-8C8E-4C217D8B4D74}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7B5F39B-10E5-4701-A025-477D215692A6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7B5F39B-10E5-4701-A025-477D215692A6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{345E4A68-49FF-4A84-8C8E-4C217D8B4D74}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f3bb3ef3-874e-4bfe-a810-81c575a8e62c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFC329E1-1AE8-4FBF-885F-BDE9D06BAFDE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFC329E1-1AE8-4FBF-885F-BDE9D06BAFDE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="f3bb3ef3-874e-4bfe-a810-81c575a8e62c"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>